<commit_message>
BD FINALE drop tABLE
</commit_message>
<xml_diff>
--- a/Base de données.xlsx
+++ b/Base de données.xlsx
@@ -145,7 +145,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,6 +155,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -315,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -329,6 +335,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -611,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,6 +680,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
+      <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -685,6 +694,7 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="5"/>
+      <c r="J3" s="13"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -698,6 +708,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="5"/>
+      <c r="J4" s="14"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -711,6 +722,7 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="5"/>
+      <c r="J5" s="13"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -724,6 +736,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="5"/>
+      <c r="J6" s="13"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -737,6 +750,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="5"/>
+      <c r="J7" s="13"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -750,6 +764,7 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="5"/>
+      <c r="J8" s="13"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -763,6 +778,7 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="5"/>
+      <c r="J9" s="13"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -776,6 +792,7 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="5"/>
+      <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -789,6 +806,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="5"/>
+      <c r="J11" s="13"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -802,6 +820,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="5"/>
+      <c r="J12" s="13"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -815,6 +834,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="5"/>
+      <c r="J13" s="13"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -828,6 +848,7 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="5"/>
+      <c r="J14" s="13"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -841,6 +862,7 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="5"/>
+      <c r="J15" s="14"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -854,8 +876,9 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="5"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="13"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>8</v>
       </c>
@@ -867,8 +890,9 @@
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="5"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="13"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>7</v>
       </c>
@@ -880,8 +904,9 @@
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="5"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="13"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>6</v>
       </c>
@@ -893,8 +918,9 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="5"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="13"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>0</v>
       </c>
@@ -906,8 +932,9 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="5"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="13"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>12</v>
       </c>
@@ -919,8 +946,9 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="5"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="13"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>13</v>
       </c>
@@ -932,8 +960,9 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="5"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="13"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
@@ -945,8 +974,9 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="5"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="13"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>9</v>
       </c>
@@ -958,8 +988,9 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="5"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="13"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>5</v>
       </c>
@@ -971,8 +1002,9 @@
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="5"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="13"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>28</v>
       </c>
@@ -984,8 +1016,9 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="5"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="13"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>10</v>
       </c>
@@ -997,8 +1030,9 @@
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="5"/>
-    </row>
-    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J27" s="13"/>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>11</v>
       </c>
@@ -1010,8 +1044,9 @@
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
       <c r="I28" s="8"/>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="J28" s="13"/>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sortState ref="A2:A28">
     <sortCondition ref="A2"/>

</xml_diff>

<commit_message>
Update avancement, maj equipes-tournois
</commit_message>
<xml_diff>
--- a/Base de données.xlsx
+++ b/Base de données.xlsx
@@ -99,9 +99,6 @@
     <t>Camisoles</t>
   </si>
   <si>
-    <t>Equipes_Tournoi</t>
-  </si>
-  <si>
     <t>Joueurs_Medicaments</t>
   </si>
   <si>
@@ -130,6 +127,9 @@
   </si>
   <si>
     <t>Dep</t>
+  </si>
+  <si>
+    <t>Equipes_Tournois</t>
   </si>
 </sst>
 </file>
@@ -619,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,7 +638,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -662,10 +662,10 @@
         <v>23</v>
       </c>
       <c r="I1" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>35</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -674,7 +674,7 @@
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
-      <c r="D2" s="4"/>
+      <c r="D2" s="9"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -688,7 +688,7 @@
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
-      <c r="D3" s="4"/>
+      <c r="D3" s="9"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -702,7 +702,7 @@
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
-      <c r="D4" s="4"/>
+      <c r="D4" s="9"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -712,11 +712,11 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
-      <c r="D5" s="4"/>
+      <c r="D5" s="9"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -730,7 +730,7 @@
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
-      <c r="D6" s="4"/>
+      <c r="D6" s="9"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -744,7 +744,7 @@
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
-      <c r="D7" s="4"/>
+      <c r="D7" s="9"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -758,7 +758,7 @@
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
-      <c r="D8" s="4"/>
+      <c r="D8" s="9"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -768,11 +768,11 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
-      <c r="D9" s="4"/>
+      <c r="D9" s="9"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -786,7 +786,7 @@
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
-      <c r="D10" s="4"/>
+      <c r="D10" s="9"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -800,7 +800,7 @@
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
-      <c r="D11" s="4"/>
+      <c r="D11" s="9"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -810,11 +810,11 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
-      <c r="D12" s="4"/>
+      <c r="D12" s="9"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -824,11 +824,11 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
-      <c r="D13" s="4"/>
+      <c r="D13" s="9"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -838,11 +838,11 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
-      <c r="D14" s="4"/>
+      <c r="D14" s="9"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -856,7 +856,7 @@
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
-      <c r="D15" s="4"/>
+      <c r="D15" s="9"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -866,11 +866,11 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
-      <c r="D16" s="4"/>
+      <c r="D16" s="9"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -884,7 +884,7 @@
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
-      <c r="D17" s="4"/>
+      <c r="D17" s="9"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -898,7 +898,7 @@
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
-      <c r="D18" s="4"/>
+      <c r="D18" s="9"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -912,7 +912,7 @@
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
-      <c r="D19" s="4"/>
+      <c r="D19" s="9"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -926,7 +926,7 @@
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
-      <c r="D20" s="4"/>
+      <c r="D20" s="9"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -940,7 +940,7 @@
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
-      <c r="D21" s="4"/>
+      <c r="D21" s="9"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -954,7 +954,7 @@
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
-      <c r="D22" s="4"/>
+      <c r="D22" s="9"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -964,11 +964,11 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
-      <c r="D23" s="4"/>
+      <c r="D23" s="9"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -982,7 +982,7 @@
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
-      <c r="D24" s="4"/>
+      <c r="D24" s="9"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
@@ -996,7 +996,7 @@
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
-      <c r="D25" s="4"/>
+      <c r="D25" s="9"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
@@ -1006,11 +1006,11 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
-      <c r="D26" s="4"/>
+      <c r="D26" s="9"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
@@ -1024,7 +1024,7 @@
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
-      <c r="D27" s="4"/>
+      <c r="D27" s="9"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
@@ -1038,7 +1038,7 @@
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
-      <c r="D28" s="7"/>
+      <c r="D28" s="10"/>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>

</xml_diff>

<commit_message>
trigger cb et update du excel
</commit_message>
<xml_diff>
--- a/Base de données.xlsx
+++ b/Base de données.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -321,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -337,6 +337,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,11 +620,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.140625" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
@@ -688,12 +689,12 @@
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-      <c r="I3" s="5"/>
+      <c r="I3" s="15"/>
       <c r="J3" s="13"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -716,12 +717,12 @@
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="5"/>
+      <c r="I5" s="15"/>
       <c r="J5" s="13"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -744,12 +745,12 @@
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="5"/>
+      <c r="I7" s="15"/>
       <c r="J7" s="13"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -758,12 +759,12 @@
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
-      <c r="I8" s="5"/>
+      <c r="I8" s="15"/>
       <c r="J8" s="13"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -786,12 +787,12 @@
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
-      <c r="I10" s="5"/>
+      <c r="I10" s="15"/>
       <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -800,12 +801,12 @@
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
-      <c r="I11" s="5"/>
+      <c r="I11" s="15"/>
       <c r="J11" s="13"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -828,12 +829,12 @@
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="5"/>
+      <c r="I13" s="15"/>
       <c r="J13" s="13"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Create Table Final non verifie
</commit_message>
<xml_diff>
--- a/Base de données.xlsx
+++ b/Base de données.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Personnes</t>
   </si>
@@ -93,15 +93,9 @@
     <t>Create Trigger Delete</t>
   </si>
   <si>
-    <t>Dispos_Entraineur</t>
-  </si>
-  <si>
     <t>Camisoles</t>
   </si>
   <si>
-    <t>Equipes_Tournoi</t>
-  </si>
-  <si>
     <t>Joueurs_Medicaments</t>
   </si>
   <si>
@@ -123,13 +117,22 @@
     <t>Inscriptions</t>
   </si>
   <si>
-    <t>Dispos_Gym</t>
-  </si>
-  <si>
     <t>Foreign Key</t>
   </si>
   <si>
     <t>Dep</t>
+  </si>
+  <si>
+    <t>Equipes_Tournois</t>
+  </si>
+  <si>
+    <t>Dispos_Gyms</t>
+  </si>
+  <si>
+    <t>Dispos_Entraineurs</t>
+  </si>
+  <si>
+    <t>Recompenses_Entraineurs</t>
   </si>
 </sst>
 </file>
@@ -145,7 +148,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,6 +167,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -321,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -340,6 +355,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,15 +638,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" customWidth="1"/>
@@ -641,7 +659,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -665,24 +683,24 @@
         <v>23</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="9"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="16"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="9"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="5"/>
+      <c r="I2" s="15"/>
       <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -691,8 +709,8 @@
       </c>
       <c r="B3" s="16"/>
       <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="16"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="9"/>
       <c r="F3" s="9"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -705,8 +723,8 @@
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="9"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="18"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -715,11 +733,11 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
+      <c r="D5" s="19"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="4"/>
@@ -729,11 +747,11 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B6" s="16"/>
       <c r="C6" s="9"/>
-      <c r="D6" s="4"/>
+      <c r="D6" s="19"/>
       <c r="E6" s="16"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -747,7 +765,7 @@
       </c>
       <c r="B7" s="16"/>
       <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
+      <c r="D7" s="19"/>
       <c r="E7" s="16"/>
       <c r="F7" s="9"/>
       <c r="G7" s="4"/>
@@ -761,7 +779,7 @@
       </c>
       <c r="B8" s="16"/>
       <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
+      <c r="D8" s="19"/>
       <c r="E8" s="16"/>
       <c r="F8" s="9"/>
       <c r="G8" s="4"/>
@@ -771,11 +789,11 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B9" s="16"/>
       <c r="C9" s="9"/>
-      <c r="D9" s="4"/>
+      <c r="D9" s="19"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -789,7 +807,7 @@
       </c>
       <c r="B10" s="16"/>
       <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
+      <c r="D10" s="19"/>
       <c r="E10" s="16"/>
       <c r="F10" s="9"/>
       <c r="G10" s="4"/>
@@ -803,7 +821,7 @@
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
+      <c r="D11" s="19"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="4"/>
@@ -813,11 +831,11 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" s="16"/>
       <c r="C12" s="9"/>
-      <c r="D12" s="4"/>
+      <c r="D12" s="19"/>
       <c r="E12" s="16"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -827,11 +845,11 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13" s="16"/>
       <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
+      <c r="D13" s="19"/>
       <c r="E13" s="16"/>
       <c r="F13" s="9"/>
       <c r="G13" s="4"/>
@@ -841,11 +859,11 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B14" s="16"/>
       <c r="C14" s="9"/>
-      <c r="D14" s="4"/>
+      <c r="D14" s="19"/>
       <c r="E14" s="16"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -859,7 +877,7 @@
       </c>
       <c r="B15" s="16"/>
       <c r="C15" s="9"/>
-      <c r="D15" s="4"/>
+      <c r="D15" s="19"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -869,11 +887,11 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B16" s="16"/>
       <c r="C16" s="9"/>
-      <c r="D16" s="4"/>
+      <c r="D16" s="19"/>
       <c r="E16" s="16"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -887,7 +905,7 @@
       </c>
       <c r="B17" s="16"/>
       <c r="C17" s="9"/>
-      <c r="D17" s="4"/>
+      <c r="D17" s="19"/>
       <c r="E17" s="16"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -901,7 +919,7 @@
       </c>
       <c r="B18" s="16"/>
       <c r="C18" s="9"/>
-      <c r="D18" s="4"/>
+      <c r="D18" s="19"/>
       <c r="E18" s="16"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -915,7 +933,7 @@
       </c>
       <c r="B19" s="16"/>
       <c r="C19" s="9"/>
-      <c r="D19" s="4"/>
+      <c r="D19" s="19"/>
       <c r="E19" s="16"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -929,7 +947,7 @@
       </c>
       <c r="B20" s="16"/>
       <c r="C20" s="9"/>
-      <c r="D20" s="4"/>
+      <c r="D20" s="19"/>
       <c r="E20" s="16"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -943,7 +961,7 @@
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="9"/>
-      <c r="D21" s="4"/>
+      <c r="D21" s="19"/>
       <c r="E21" s="16"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -957,7 +975,7 @@
       </c>
       <c r="B22" s="16"/>
       <c r="C22" s="9"/>
-      <c r="D22" s="4"/>
+      <c r="D22" s="19"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -967,11 +985,11 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B23" s="16"/>
       <c r="C23" s="9"/>
-      <c r="D23" s="4"/>
+      <c r="D23" s="19"/>
       <c r="E23" s="16"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -985,7 +1003,7 @@
       </c>
       <c r="B24" s="16"/>
       <c r="C24" s="9"/>
-      <c r="D24" s="4"/>
+      <c r="D24" s="19"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
@@ -995,11 +1013,11 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="16"/>
+        <v>37</v>
+      </c>
+      <c r="B25" s="18"/>
       <c r="C25" s="9"/>
-      <c r="D25" s="4"/>
+      <c r="D25" s="19"/>
       <c r="E25" s="16"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
@@ -1009,11 +1027,11 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="B26" s="16"/>
       <c r="C26" s="9"/>
-      <c r="D26" s="4"/>
+      <c r="D26" s="19"/>
       <c r="E26" s="16"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
@@ -1023,11 +1041,11 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B27" s="16"/>
       <c r="C27" s="9"/>
-      <c r="D27" s="4"/>
+      <c r="D27" s="19"/>
       <c r="E27" s="16"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
@@ -1035,21 +1053,35 @@
       <c r="I27" s="5"/>
       <c r="J27" s="13"/>
     </row>
-    <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="16"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="13"/>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="13"/>
-    </row>
-    <row r="29" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="13"/>
+    </row>
+    <row r="30" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sortState ref="A2:A28">
     <sortCondition ref="A2"/>

</xml_diff>